<commit_message>
updated gantt chart with dates and added those dates to proj definition
</commit_message>
<xml_diff>
--- a/Msc Proj Gantt Chart.xlsx
+++ b/Msc Proj Gantt Chart.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Copy this file to edit this chart. Go to File, the select "Make a Copy". Please don't Request Access</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Project Definition Document</t>
   </si>
   <si>
+    <t>22/2/2021</t>
+  </si>
+  <si>
     <t>Topic Background Research</t>
   </si>
   <si>
@@ -71,6 +74,12 @@
   </si>
   <si>
     <t>Dataset Investigation</t>
+  </si>
+  <si>
+    <t>15/3/2021</t>
+  </si>
+  <si>
+    <t>29/3/2021</t>
   </si>
   <si>
     <t>Dataset Selection</t>
@@ -91,6 +100,9 @@
     <t>Expand Model To Include Subclasses</t>
   </si>
   <si>
+    <t>28/6/2021</t>
+  </si>
+  <si>
     <t>Laurie Strode</t>
   </si>
   <si>
@@ -103,19 +115,37 @@
     <t>Abstract</t>
   </si>
   <si>
+    <t>19/4/2021</t>
+  </si>
+  <si>
+    <t>17/5/2021</t>
+  </si>
+  <si>
     <t>Andy Barclay</t>
   </si>
   <si>
     <t>Introduction</t>
   </si>
   <si>
+    <t>31/5/2021</t>
+  </si>
+  <si>
     <t>Background / Related Work</t>
+  </si>
+  <si>
+    <t>22/3/2021</t>
   </si>
   <si>
     <t>Methodology</t>
   </si>
   <si>
     <t>Experiments / Results</t>
+  </si>
+  <si>
+    <t>21/6/2021</t>
+  </si>
+  <si>
+    <t>19/7/2021</t>
   </si>
   <si>
     <t>Jason Myers</t>
@@ -150,7 +180,7 @@
     <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -206,6 +236,10 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -249,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -299,6 +333,12 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -317,10 +357,16 @@
     <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -400,11 +446,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1136940137"/>
-        <c:axId val="1127913598"/>
+        <c:axId val="1829608290"/>
+        <c:axId val="193858893"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1136940137"/>
+        <c:axId val="1829608290"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -456,10 +502,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1127913598"/>
+        <c:crossAx val="193858893"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1127913598"/>
+        <c:axId val="193858893"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -535,7 +581,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1136940137"/>
+        <c:crossAx val="1829608290"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -988,10 +1034,14 @@
         <v>14</v>
       </c>
       <c r="C6" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>44410.0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="14">
         <f>INT(D6)-INT($D$6)</f>
         <v>0</v>
@@ -1000,18 +1050,18 @@
         <v>2.0</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="13">
+      <c r="I6" s="17">
         <v>25.0</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="17">
         <v>28.0</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="13">
+      <c r="M6" s="17">
         <v>5.0</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="17">
         <v>4.0</v>
       </c>
       <c r="X6" s="4"/>
@@ -1024,13 +1074,17 @@
     <row r="7">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="11">
         <v>0.0</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="18">
+        <v>44411.0</v>
+      </c>
       <c r="F7" s="15">
         <v>2.0</v>
       </c>
@@ -1038,20 +1092,20 @@
         <v>4.0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="13">
+        <v>17</v>
+      </c>
+      <c r="I7" s="17">
         <v>15.0</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="17">
         <v>20.0</v>
       </c>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="13">
+      <c r="M7" s="17">
         <v>5.0</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="17">
         <v>4.0</v>
       </c>
       <c r="X7" s="4"/>
@@ -1070,17 +1124,17 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="13">
+        <v>18</v>
+      </c>
+      <c r="I8" s="17">
         <v>10.0</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="17">
         <v>8.0</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="13">
+      <c r="M8" s="17">
         <v>5.0</v>
       </c>
       <c r="N8" s="16"/>
@@ -1093,31 +1147,31 @@
     </row>
     <row r="9">
       <c r="A9" s="10"/>
-      <c r="B9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21">
+      <c r="B9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23">
         <v>95.0</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="23">
         <v>84.0</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="23">
         <v>1600.0</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="23">
         <v>1550.0</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="23">
         <v>4.0</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="23">
         <v>2.0</v>
       </c>
       <c r="X9" s="4"/>
@@ -1130,34 +1184,38 @@
     <row r="10">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="11">
         <v>0.0</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="22">
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="24">
         <v>5.0</v>
       </c>
       <c r="G10" s="15">
         <v>2.0</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="13">
+        <v>18</v>
+      </c>
+      <c r="I10" s="17">
         <v>2.0</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="17">
         <v>2.0</v>
       </c>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="13">
+      <c r="M10" s="17">
         <v>4.0</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="17">
         <v>2.0</v>
       </c>
       <c r="X10" s="4"/>
@@ -1170,38 +1228,42 @@
     <row r="11">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" s="11">
         <v>0.0</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="22">
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="18">
+        <v>44320.0</v>
+      </c>
+      <c r="F11" s="24">
         <v>7.0</v>
       </c>
       <c r="G11" s="15">
         <v>1.0</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="13">
+        <v>24</v>
+      </c>
+      <c r="I11" s="17">
         <v>48.0</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="17">
         <v>40.0</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="17">
         <v>500.0</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="17">
         <v>450.0</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="17">
         <v>3.0</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="17">
         <v>2.0</v>
       </c>
       <c r="X11" s="4"/>
@@ -1214,38 +1276,42 @@
     <row r="12">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" s="11">
         <v>0.0</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="22">
+      <c r="D12" s="12">
+        <v>44320.0</v>
+      </c>
+      <c r="E12" s="12">
+        <v>44534.0</v>
+      </c>
+      <c r="F12" s="24">
         <v>8.0</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="13">
+        <v>17</v>
+      </c>
+      <c r="I12" s="17">
         <v>45.0</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="17">
         <v>42.0</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="17">
         <v>300.0</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="17">
         <v>325.0</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="17">
         <v>2.0</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="17">
         <v>1.0</v>
       </c>
       <c r="X12" s="4"/>
@@ -1260,24 +1326,24 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="14"/>
       <c r="H13" s="10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
-      <c r="K13" s="13">
+      <c r="K13" s="17">
         <v>800.0</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="17">
         <v>775.0</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="17">
         <v>5.0</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="17">
         <v>2.0</v>
       </c>
       <c r="X13" s="4"/>
@@ -1289,31 +1355,31 @@
     </row>
     <row r="14">
       <c r="A14" s="10"/>
-      <c r="B14" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21">
+      <c r="B14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23">
         <v>112.0</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="23">
         <v>98.0</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="23">
         <v>350.0</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="23">
         <v>250.0</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="23">
         <v>4.0</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="23">
         <v>3.0</v>
       </c>
       <c r="X14" s="4"/>
@@ -1326,38 +1392,42 @@
     <row r="15">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15" s="11">
         <v>0.0</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="22">
+      <c r="D15" s="18">
+        <v>44534.0</v>
+      </c>
+      <c r="E15" s="25">
+        <v>44383.0</v>
+      </c>
+      <c r="F15" s="24">
         <v>9.0</v>
       </c>
       <c r="G15" s="15">
         <v>8.0</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="13">
+        <v>17</v>
+      </c>
+      <c r="I15" s="17">
         <v>72.0</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="17">
         <v>72.0</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="17">
         <v>350.0</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="17">
         <v>250.0</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="17">
         <v>5.0</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="17">
         <v>5.0</v>
       </c>
       <c r="X15" s="4"/>
@@ -1370,34 +1440,38 @@
     <row r="16">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C16" s="11">
         <v>0.0</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="22">
+      <c r="D16" s="18">
+        <v>44260.0</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="24">
         <v>12.0</v>
       </c>
       <c r="G16" s="15">
         <v>8.0</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="13">
+        <v>30</v>
+      </c>
+      <c r="I16" s="17">
         <v>36.0</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="17">
         <v>24.0</v>
       </c>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
-      <c r="M16" s="13">
+      <c r="M16" s="17">
         <v>3.0</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="17">
         <v>3.0</v>
       </c>
       <c r="X16" s="4"/>
@@ -1410,34 +1484,38 @@
     <row r="17">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C17" s="11">
         <v>0.0</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="22">
+      <c r="D17" s="18">
+        <v>44534.0</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="24">
         <v>9.0</v>
       </c>
       <c r="G17" s="15">
         <v>11.0</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="13">
+        <v>17</v>
+      </c>
+      <c r="I17" s="17">
         <v>4.0</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="17">
         <v>2.0</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="13">
+      <c r="M17" s="17">
         <v>5.0</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="17">
         <v>1.0</v>
       </c>
       <c r="X17" s="4"/>
@@ -1449,27 +1527,27 @@
     </row>
     <row r="18">
       <c r="A18" s="10"/>
-      <c r="B18" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="21">
+      <c r="B18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23">
         <v>28.0</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="23">
         <v>28.0</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21">
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23">
         <v>4.0</v>
       </c>
-      <c r="N18" s="20"/>
+      <c r="N18" s="22"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
@@ -1480,31 +1558,35 @@
     <row r="19">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C19" s="11">
         <v>0.0</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22">
+      <c r="D19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="24">
         <v>10.0</v>
       </c>
       <c r="G19" s="15">
         <v>4.0</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="13">
+        <v>36</v>
+      </c>
+      <c r="I19" s="17">
         <v>5.0</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="17">
         <v>4.0</v>
       </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="13">
+      <c r="M19" s="17">
         <v>5.0</v>
       </c>
       <c r="N19" s="16"/>
@@ -1518,31 +1600,35 @@
     <row r="20">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C20" s="11">
         <v>0.0</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="22">
+      <c r="D20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="24">
         <v>14.0</v>
       </c>
       <c r="G20" s="15">
         <v>2.0</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="13">
+        <v>24</v>
+      </c>
+      <c r="I20" s="17">
         <v>10.0</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="17">
         <v>10.0</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="13">
+      <c r="M20" s="17">
         <v>5.0</v>
       </c>
       <c r="N20" s="16"/>
@@ -1556,31 +1642,35 @@
     <row r="21">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11">
         <v>0.0</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="22">
+      <c r="D21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="24">
         <v>6.0</v>
       </c>
       <c r="G21" s="15">
         <v>14.0</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="13">
+        <v>17</v>
+      </c>
+      <c r="I21" s="17">
         <v>10.0</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="17">
         <v>12.0</v>
       </c>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="13">
+      <c r="M21" s="17">
         <v>5.0</v>
       </c>
       <c r="N21" s="16"/>
@@ -1594,31 +1684,35 @@
     <row r="22">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C22" s="11">
         <v>0.0</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="22">
+      <c r="D22" s="18">
+        <v>44534.0</v>
+      </c>
+      <c r="E22" s="18">
+        <v>44323.0</v>
+      </c>
+      <c r="F22" s="24">
         <v>9.0</v>
       </c>
       <c r="G22" s="15">
         <v>12.0</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="13">
+        <v>17</v>
+      </c>
+      <c r="I22" s="17">
         <v>1.0</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="17">
         <v>0.5</v>
       </c>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="13">
+      <c r="M22" s="17">
         <v>2.0</v>
       </c>
       <c r="N22" s="16"/>
@@ -1632,31 +1726,35 @@
     <row r="23">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C23" s="11">
         <v>0.0</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22">
+      <c r="D23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="24">
         <v>19.0</v>
       </c>
       <c r="G23" s="15">
         <v>4.0</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="13">
+        <v>45</v>
+      </c>
+      <c r="I23" s="17">
         <v>1.0</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="17">
         <v>1.0</v>
       </c>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
-      <c r="M23" s="13">
+      <c r="M23" s="17">
         <v>5.0</v>
       </c>
       <c r="N23" s="16"/>
@@ -1670,31 +1768,35 @@
     <row r="24">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C24" s="11">
         <v>0.0</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="22">
+      <c r="D24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="24">
         <v>20.0</v>
       </c>
       <c r="G24" s="15">
         <v>3.0</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="13">
+        <v>17</v>
+      </c>
+      <c r="I24" s="17">
         <v>1.0</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="17">
         <v>0.5</v>
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
-      <c r="M24" s="13">
+      <c r="M24" s="17">
         <v>3.0</v>
       </c>
       <c r="N24" s="16"/>
@@ -1707,31 +1809,31 @@
     </row>
     <row r="25">
       <c r="A25" s="10"/>
-      <c r="B25" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21">
+      <c r="B25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23">
         <v>53.0</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="23">
         <v>50.0</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="23">
         <v>855.0</v>
       </c>
-      <c r="L25" s="21">
+      <c r="L25" s="23">
         <v>655.0</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="23">
         <v>4.0</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="23">
         <v>3.0</v>
       </c>
       <c r="X25" s="4"/>
@@ -1744,38 +1846,42 @@
     <row r="26">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C26" s="11">
         <v>0.0</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="22">
+      <c r="D26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="18">
+        <v>44447.0</v>
+      </c>
+      <c r="F26" s="24">
         <v>23.0</v>
       </c>
       <c r="G26" s="15">
         <v>4.0</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="13">
+        <v>30</v>
+      </c>
+      <c r="I26" s="17">
         <v>10.0</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="17">
         <v>9.0</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="17">
         <v>200.0</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="17">
         <v>150.0</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="17">
         <v>5.0</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="17">
         <v>3.0</v>
       </c>
       <c r="X26" s="4"/>
@@ -1788,38 +1894,42 @@
     <row r="27">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C27" s="11">
         <v>0.0</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="22">
+      <c r="D27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="18">
+        <v>44447.0</v>
+      </c>
+      <c r="F27" s="24">
         <v>23.0</v>
       </c>
       <c r="G27" s="15">
         <v>4.0</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="13">
+        <v>17</v>
+      </c>
+      <c r="I27" s="17">
         <v>15.0</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="17">
         <v>10.0</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="17">
         <v>450.0</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="17">
         <v>300.0</v>
       </c>
-      <c r="M27" s="13">
+      <c r="M27" s="17">
         <v>4.0</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="17">
         <v>1.0</v>
       </c>
       <c r="X27" s="4"/>
@@ -1832,35 +1942,39 @@
     <row r="28">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C28" s="11">
         <v>0.0</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="22">
+      <c r="D28" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="18">
+        <v>44447.0</v>
+      </c>
+      <c r="F28" s="24">
         <v>23.0</v>
       </c>
       <c r="G28" s="15">
         <v>4.0</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="13">
+        <v>24</v>
+      </c>
+      <c r="I28" s="17">
         <v>20.0</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="17">
         <v>24.0</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="17">
         <v>100.0</v>
       </c>
-      <c r="L28" s="13">
+      <c r="L28" s="17">
         <v>100.0</v>
       </c>
-      <c r="M28" s="13">
+      <c r="M28" s="17">
         <v>3.0</v>
       </c>
       <c r="N28" s="16"/>
@@ -1875,17 +1989,17 @@
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="22"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
       <c r="H29" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="13">
+        <v>18</v>
+      </c>
+      <c r="I29" s="17">
         <v>1.0</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="17">
         <v>1.0</v>
       </c>
       <c r="K29" s="16"/>
@@ -1903,29 +2017,29 @@
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="22"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="14"/>
       <c r="H30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="13">
+        <v>17</v>
+      </c>
+      <c r="I30" s="17">
         <v>5.0</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="17">
         <v>4.0</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="17">
         <v>105.0</v>
       </c>
-      <c r="L30" s="13">
+      <c r="L30" s="17">
         <v>105.0</v>
       </c>
-      <c r="M30" s="13">
+      <c r="M30" s="17">
         <v>5.0</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="17">
         <v>4.0</v>
       </c>
       <c r="X30" s="4"/>
@@ -1939,17 +2053,17 @@
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="22"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="14"/>
       <c r="H31" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="13">
+        <v>18</v>
+      </c>
+      <c r="I31" s="17">
         <v>1.0</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="17">
         <v>1.0</v>
       </c>
       <c r="K31" s="16"/>
@@ -1967,17 +2081,17 @@
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="22"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="14"/>
       <c r="H32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="13">
+        <v>18</v>
+      </c>
+      <c r="I32" s="17">
         <v>1.0</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="17">
         <v>1.0</v>
       </c>
       <c r="K32" s="16"/>
@@ -1993,29 +2107,29 @@
     </row>
     <row r="33">
       <c r="A33" s="10"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21">
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23">
         <v>9.5</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="23">
         <v>9.5</v>
       </c>
-      <c r="K33" s="21">
+      <c r="K33" s="23">
         <v>100.0</v>
       </c>
-      <c r="L33" s="21">
+      <c r="L33" s="23">
         <v>150.0</v>
       </c>
-      <c r="M33" s="21">
+      <c r="M33" s="23">
         <v>4.0</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="23">
         <v>3.0</v>
       </c>
       <c r="X33" s="4"/>
@@ -2029,29 +2143,29 @@
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="22"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="24"/>
       <c r="G34" s="14"/>
       <c r="H34" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" s="13">
+        <v>45</v>
+      </c>
+      <c r="I34" s="17">
         <v>3.0</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="17">
         <v>3.0</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="17">
         <v>100.0</v>
       </c>
-      <c r="L34" s="13">
+      <c r="L34" s="17">
         <v>150.0</v>
       </c>
-      <c r="M34" s="13">
+      <c r="M34" s="17">
         <v>4.0</v>
       </c>
-      <c r="N34" s="13">
+      <c r="N34" s="17">
         <v>3.0</v>
       </c>
       <c r="X34" s="4"/>
@@ -2065,17 +2179,17 @@
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="22"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="24"/>
       <c r="G35" s="14"/>
       <c r="H35" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="13">
+        <v>45</v>
+      </c>
+      <c r="I35" s="17">
         <v>1.0</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="17">
         <v>1.0</v>
       </c>
       <c r="K35" s="16"/>
@@ -2093,25 +2207,25 @@
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="22"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="24"/>
       <c r="G36" s="14"/>
       <c r="H36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="13">
+        <v>17</v>
+      </c>
+      <c r="I36" s="17">
         <v>1.0</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="17">
         <v>1.0</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
-      <c r="M36" s="13">
+      <c r="M36" s="17">
         <v>4.0</v>
       </c>
-      <c r="N36" s="13">
+      <c r="N36" s="17">
         <v>4.0</v>
       </c>
       <c r="X36" s="4"/>
@@ -2125,25 +2239,25 @@
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="22"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="24"/>
       <c r="G37" s="14"/>
       <c r="H37" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I37" s="13">
+        <v>51</v>
+      </c>
+      <c r="I37" s="17">
         <v>0.5</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="17">
         <v>0.5</v>
       </c>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
-      <c r="M37" s="13">
+      <c r="M37" s="17">
         <v>4.0</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N37" s="17">
         <v>1.0</v>
       </c>
       <c r="X37" s="4"/>
@@ -2157,29 +2271,29 @@
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="22"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="24"/>
       <c r="G38" s="14"/>
       <c r="H38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="13">
+        <v>17</v>
+      </c>
+      <c r="I38" s="17">
         <v>4.0</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="17">
         <v>3.0</v>
       </c>
-      <c r="K38" s="13">
+      <c r="K38" s="17">
         <v>150.0</v>
       </c>
-      <c r="L38" s="13">
+      <c r="L38" s="17">
         <v>200.0</v>
       </c>
-      <c r="M38" s="13">
+      <c r="M38" s="17">
         <v>5.0</v>
       </c>
-      <c r="N38" s="13">
+      <c r="N38" s="17">
         <v>2.0</v>
       </c>
       <c r="X38" s="4"/>
@@ -2193,27 +2307,27 @@
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="22"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="24"/>
       <c r="G39" s="14"/>
       <c r="H39" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="13">
+        <v>18</v>
+      </c>
+      <c r="I39" s="17">
         <v>15.0</v>
       </c>
       <c r="J39" s="16"/>
-      <c r="K39" s="13">
+      <c r="K39" s="17">
         <v>250.0</v>
       </c>
-      <c r="L39" s="13">
+      <c r="L39" s="17">
         <v>250.0</v>
       </c>
-      <c r="M39" s="13">
+      <c r="M39" s="17">
         <v>5.0</v>
       </c>
-      <c r="N39" s="13">
+      <c r="N39" s="17">
         <v>1.0</v>
       </c>
       <c r="X39" s="4"/>
@@ -2227,14 +2341,14 @@
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="22"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="24"/>
       <c r="G40" s="14"/>
       <c r="H40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="13">
+        <v>24</v>
+      </c>
+      <c r="I40" s="17">
         <v>2.0</v>
       </c>
       <c r="J40" s="16"/>
@@ -2253,23 +2367,23 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="22"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="24"/>
       <c r="G41" s="14"/>
       <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="13">
+        <v>36</v>
+      </c>
+      <c r="I41" s="17">
         <v>1.0</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
-      <c r="M41" s="13">
+      <c r="M41" s="17">
         <v>5.0</v>
       </c>
-      <c r="N41" s="13">
+      <c r="N41" s="17">
         <v>1.0</v>
       </c>
       <c r="X41" s="4"/>
@@ -2280,9 +2394,9 @@
       <c r="AC41" s="4"/>
     </row>
     <row r="42">
-      <c r="E42" s="24"/>
-      <c r="F42" s="13" t="s">
-        <v>42</v>
+      <c r="E42" s="28"/>
+      <c r="F42" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="G42" s="16"/>
       <c r="X42" s="4"/>
@@ -2293,7 +2407,7 @@
       <c r="AC42" s="4"/>
     </row>
     <row r="43">
-      <c r="F43" s="13"/>
+      <c r="F43" s="17"/>
       <c r="G43" s="16"/>
       <c r="X43" s="4"/>
       <c r="Y43" s="4"/>
@@ -2303,7 +2417,7 @@
       <c r="AC43" s="4"/>
     </row>
     <row r="44">
-      <c r="F44" s="13"/>
+      <c r="F44" s="17"/>
       <c r="G44" s="16"/>
       <c r="X44" s="4"/>
       <c r="Y44" s="4"/>
@@ -2313,7 +2427,7 @@
       <c r="AC44" s="4"/>
     </row>
     <row r="45">
-      <c r="F45" s="13"/>
+      <c r="F45" s="17"/>
       <c r="G45" s="16"/>
       <c r="X45" s="4"/>
       <c r="Y45" s="4"/>
@@ -2323,7 +2437,7 @@
       <c r="AC45" s="4"/>
     </row>
     <row r="46">
-      <c r="F46" s="13"/>
+      <c r="F46" s="17"/>
       <c r="G46" s="16"/>
       <c r="X46" s="4"/>
       <c r="Y46" s="4"/>
@@ -2333,7 +2447,7 @@
       <c r="AC46" s="4"/>
     </row>
     <row r="47">
-      <c r="F47" s="13"/>
+      <c r="F47" s="17"/>
       <c r="G47" s="16"/>
       <c r="X47" s="4"/>
       <c r="Y47" s="4"/>

</xml_diff>